<commit_message>
Moved some files around, finished the main Import to Odoo code, ScrapeJLCtoOdoo in progress but close
</commit_message>
<xml_diff>
--- a/jlc-scraper/csv/Parts Inventory on JLCPCB.xlsx
+++ b/jlc-scraper/csv/Parts Inventory on JLCPCB.xlsx
@@ -97,7 +97,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G154"/>
+  <dimension ref="A1:G160"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -202,7 +202,7 @@
         </is>
       </c>
       <c r="E3" s="2" t="n">
-        <v>10000.0</v>
+        <v>9615.0</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>0.0</v>
@@ -326,7 +326,7 @@
         </is>
       </c>
       <c r="E7" s="2" t="n">
-        <v>3000.0</v>
+        <v>1740.0</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>0.0</v>
@@ -357,7 +357,7 @@
         </is>
       </c>
       <c r="E8" s="2" t="n">
-        <v>4480.0</v>
+        <v>3220.0</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>0.0</v>
@@ -388,7 +388,7 @@
         </is>
       </c>
       <c r="E9" s="2" t="n">
-        <v>10000.0</v>
+        <v>9115.0</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>0.0</v>
@@ -574,7 +574,7 @@
         </is>
       </c>
       <c r="E15" s="2" t="n">
-        <v>100.0</v>
+        <v>200.0</v>
       </c>
       <c r="F15" s="2" t="n">
         <v>0.0</v>
@@ -946,7 +946,7 @@
         </is>
       </c>
       <c r="E27" s="2" t="n">
-        <v>1000.0</v>
+        <v>865.0</v>
       </c>
       <c r="F27" s="2" t="n">
         <v>0.0</v>
@@ -1008,7 +1008,7 @@
         </is>
       </c>
       <c r="E29" s="2" t="n">
-        <v>1000.0</v>
+        <v>2000.0</v>
       </c>
       <c r="F29" s="2" t="n">
         <v>0.0</v>
@@ -1318,7 +1318,7 @@
         </is>
       </c>
       <c r="E39" s="2" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="F39" s="2" t="n">
         <v>0.0</v>
@@ -1485,22 +1485,22 @@
     <row r="45">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>Inductors, Coils, Chokes</t>
+          <t>Resistors</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
         <is>
-          <t>QT48A03</t>
+          <t>AF0201JR-0720RL</t>
         </is>
       </c>
       <c r="C45" s="2" t="inlineStr">
         <is>
-          <t>SMD</t>
+          <t>0201</t>
         </is>
       </c>
       <c r="D45" s="2" t="inlineStr">
         <is>
-          <t>C216365</t>
+          <t>C2101262</t>
         </is>
       </c>
       <c r="E45" s="2" t="n">
@@ -1510,7 +1510,7 @@
         <v>0.0</v>
       </c>
       <c r="G45" s="2" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="46">
@@ -1521,7 +1521,7 @@
       </c>
       <c r="B46" s="2" t="inlineStr">
         <is>
-          <t>AC0201FR-07120RL</t>
+          <t>AF0201FR-076K49L</t>
         </is>
       </c>
       <c r="C46" s="2" t="inlineStr">
@@ -1531,11 +1531,11 @@
       </c>
       <c r="D46" s="2" t="inlineStr">
         <is>
-          <t>C226406</t>
+          <t>C2107920</t>
         </is>
       </c>
       <c r="E46" s="2" t="n">
-        <v>7025.0</v>
+        <v>0.0</v>
       </c>
       <c r="F46" s="2" t="n">
         <v>0.0</v>
@@ -1547,57 +1547,57 @@
     <row r="47">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>Capacitors</t>
+          <t>Inductors, Coils, Chokes</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
         <is>
-          <t>CC1206KKX7RDBB102</t>
+          <t>QT48A03</t>
         </is>
       </c>
       <c r="C47" s="2" t="inlineStr">
         <is>
-          <t>1206</t>
+          <t>SMD</t>
         </is>
       </c>
       <c r="D47" s="2" t="inlineStr">
         <is>
-          <t>C23631</t>
+          <t>C216365</t>
         </is>
       </c>
       <c r="E47" s="2" t="n">
-        <v>3000.0</v>
+        <v>0.0</v>
       </c>
       <c r="F47" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="G47" s="2" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>Diodes</t>
+          <t>Resistors</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
         <is>
-          <t>MBR0520LT1G</t>
+          <t>AC0201FR-07120RL</t>
         </is>
       </c>
       <c r="C48" s="2" t="inlineStr">
         <is>
-          <t>SOD-123</t>
+          <t>0201</t>
         </is>
       </c>
       <c r="D48" s="2" t="inlineStr">
         <is>
-          <t>C23848</t>
+          <t>C226406</t>
         </is>
       </c>
       <c r="E48" s="2" t="n">
-        <v>0.0</v>
+        <v>7025.0</v>
       </c>
       <c r="F48" s="2" t="n">
         <v>0.0</v>
@@ -1609,26 +1609,26 @@
     <row r="49">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>Circuit Protection</t>
+          <t>Capacitors</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
         <is>
-          <t>PJGBLC12C_R1_00001</t>
+          <t>CC1206KKX7RDBB102</t>
         </is>
       </c>
       <c r="C49" s="2" t="inlineStr">
         <is>
-          <t>SOD-323</t>
+          <t>1206</t>
         </is>
       </c>
       <c r="D49" s="2" t="inlineStr">
         <is>
-          <t>C263347</t>
+          <t>C23631</t>
         </is>
       </c>
       <c r="E49" s="2" t="n">
-        <v>200.0</v>
+        <v>3000.0</v>
       </c>
       <c r="F49" s="2" t="n">
         <v>0.0</v>
@@ -1640,22 +1640,22 @@
     <row r="50">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>Capacitors</t>
+          <t>Diodes</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
         <is>
-          <t>GRM155R71H104KE14J</t>
+          <t>MBR0520LT1G</t>
         </is>
       </c>
       <c r="C50" s="2" t="inlineStr">
         <is>
-          <t>0402</t>
+          <t>SOD-123</t>
         </is>
       </c>
       <c r="D50" s="2" t="inlineStr">
         <is>
-          <t>C2649519</t>
+          <t>C23848</t>
         </is>
       </c>
       <c r="E50" s="2" t="n">
@@ -1671,26 +1671,26 @@
     <row r="51">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>Capacitors</t>
+          <t>Circuit Protection</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
         <is>
-          <t>GRM033R61E104KE14J</t>
+          <t>PJGBLC12C_R1_00001</t>
         </is>
       </c>
       <c r="C51" s="2" t="inlineStr">
         <is>
-          <t>0201</t>
+          <t>SOD-323</t>
         </is>
       </c>
       <c r="D51" s="2" t="inlineStr">
         <is>
-          <t>C2649540</t>
+          <t>C263347</t>
         </is>
       </c>
       <c r="E51" s="2" t="n">
-        <v>5000.0</v>
+        <v>200.0</v>
       </c>
       <c r="F51" s="2" t="n">
         <v>0.0</v>
@@ -1702,29 +1702,29 @@
     <row r="52">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>Resistors</t>
+          <t>Capacitors</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
         <is>
-          <t>EXB-28V221JX</t>
+          <t>GRM155R71H104KE14J</t>
         </is>
       </c>
       <c r="C52" s="2" t="inlineStr">
         <is>
-          <t>0402x4</t>
+          <t>0402</t>
         </is>
       </c>
       <c r="D52" s="2" t="inlineStr">
         <is>
-          <t>C2654090</t>
+          <t>C2649519</t>
         </is>
       </c>
       <c r="E52" s="2" t="n">
-        <v>217.0</v>
+        <v>0.0</v>
       </c>
       <c r="F52" s="2" t="n">
-        <v>2540.0</v>
+        <v>0.0</v>
       </c>
       <c r="G52" s="2" t="n">
         <v>0.0</v>
@@ -1733,29 +1733,29 @@
     <row r="53">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>Magnetic Sensors</t>
+          <t>Capacitors</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
         <is>
-          <t>AK09915C</t>
+          <t>GRM033R61E104KE14J</t>
         </is>
       </c>
       <c r="C53" s="2" t="inlineStr">
         <is>
-          <t>WLCSP-14(1.6x1.6)</t>
+          <t>0201</t>
         </is>
       </c>
       <c r="D53" s="2" t="inlineStr">
         <is>
-          <t>C2654982</t>
+          <t>C2649540</t>
         </is>
       </c>
       <c r="E53" s="2" t="n">
-        <v>0.0</v>
+        <v>5000.0</v>
       </c>
       <c r="F53" s="2" t="n">
-        <v>500.0</v>
+        <v>0.0</v>
       </c>
       <c r="G53" s="2" t="n">
         <v>0.0</v>
@@ -1769,24 +1769,24 @@
       </c>
       <c r="B54" s="2" t="inlineStr">
         <is>
-          <t>0201WMF6041TEE</t>
+          <t>EXB-28V221JX</t>
         </is>
       </c>
       <c r="C54" s="2" t="inlineStr">
         <is>
-          <t>0201</t>
+          <t>0402x4</t>
         </is>
       </c>
       <c r="D54" s="2" t="inlineStr">
         <is>
-          <t>C270341</t>
+          <t>C2654090</t>
         </is>
       </c>
       <c r="E54" s="2" t="n">
-        <v>8962.0</v>
+        <v>217.0</v>
       </c>
       <c r="F54" s="2" t="n">
-        <v>0.0</v>
+        <v>2540.0</v>
       </c>
       <c r="G54" s="2" t="n">
         <v>0.0</v>
@@ -1795,29 +1795,29 @@
     <row r="55">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>Resistors</t>
+          <t>Magnetic Sensors</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
         <is>
-          <t>0201WMF2400TEE</t>
+          <t>AK09915C</t>
         </is>
       </c>
       <c r="C55" s="2" t="inlineStr">
         <is>
-          <t>0201</t>
+          <t>WLCSP-14(1.6x1.6)</t>
         </is>
       </c>
       <c r="D55" s="2" t="inlineStr">
         <is>
-          <t>C270354</t>
+          <t>C2654982</t>
         </is>
       </c>
       <c r="E55" s="2" t="n">
-        <v>10000.0</v>
+        <v>0.0</v>
       </c>
       <c r="F55" s="2" t="n">
-        <v>0.0</v>
+        <v>500.0</v>
       </c>
       <c r="G55" s="2" t="n">
         <v>0.0</v>
@@ -1831,21 +1831,21 @@
       </c>
       <c r="B56" s="2" t="inlineStr">
         <is>
-          <t>RC0402FR-074K32L</t>
+          <t>0201WMF6041TEE</t>
         </is>
       </c>
       <c r="C56" s="2" t="inlineStr">
         <is>
-          <t>0402</t>
+          <t>0201</t>
         </is>
       </c>
       <c r="D56" s="2" t="inlineStr">
         <is>
-          <t>C273329</t>
+          <t>C270341</t>
         </is>
       </c>
       <c r="E56" s="2" t="n">
-        <v>9980.0</v>
+        <v>8962.0</v>
       </c>
       <c r="F56" s="2" t="n">
         <v>0.0</v>
@@ -1857,26 +1857,26 @@
     <row r="57">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>Capacitors</t>
+          <t>Resistors</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
         <is>
-          <t>CL10A226MO7JZNC</t>
+          <t>0201WMF2400TEE</t>
         </is>
       </c>
       <c r="C57" s="2" t="inlineStr">
         <is>
-          <t>0603</t>
+          <t>0201</t>
         </is>
       </c>
       <c r="D57" s="2" t="inlineStr">
         <is>
-          <t>C2762594</t>
+          <t>C270354</t>
         </is>
       </c>
       <c r="E57" s="2" t="n">
-        <v>1000.0</v>
+        <v>10000.0</v>
       </c>
       <c r="F57" s="2" t="n">
         <v>0.0</v>
@@ -1893,7 +1893,7 @@
       </c>
       <c r="B58" s="2" t="inlineStr">
         <is>
-          <t>RC0402FR-0731K6L</t>
+          <t>RC0402FR-074K32L</t>
         </is>
       </c>
       <c r="C58" s="2" t="inlineStr">
@@ -1903,11 +1903,11 @@
       </c>
       <c r="D58" s="2" t="inlineStr">
         <is>
-          <t>C276265</t>
+          <t>C273329</t>
         </is>
       </c>
       <c r="E58" s="2" t="n">
-        <v>0.0</v>
+        <v>9980.0</v>
       </c>
       <c r="F58" s="2" t="n">
         <v>0.0</v>
@@ -1919,26 +1919,26 @@
     <row r="59">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>Inductors, Coils, Chokes</t>
+          <t>Interface</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
         <is>
-          <t>G48C01S</t>
+          <t>RTL8367RB-VB-CG</t>
         </is>
       </c>
       <c r="C59" s="2" t="inlineStr">
         <is>
-          <t>SMD</t>
+          <t>LQFP-128</t>
         </is>
       </c>
       <c r="D59" s="2" t="inlineStr">
         <is>
-          <t>C2827284</t>
+          <t>C2761412</t>
         </is>
       </c>
       <c r="E59" s="2" t="n">
-        <v>280.0</v>
+        <v>90.0</v>
       </c>
       <c r="F59" s="2" t="n">
         <v>0.0</v>
@@ -1950,26 +1950,26 @@
     <row r="60">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>Diodes</t>
+          <t>Capacitors</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
         <is>
-          <t>LMSZ5265BT1G</t>
+          <t>CL10A226MO7JZNC</t>
         </is>
       </c>
       <c r="C60" s="2" t="inlineStr">
         <is>
-          <t>SOD-123</t>
+          <t>0603</t>
         </is>
       </c>
       <c r="D60" s="2" t="inlineStr">
         <is>
-          <t>C2847461</t>
+          <t>C2762594</t>
         </is>
       </c>
       <c r="E60" s="2" t="n">
-        <v>272.0</v>
+        <v>1000.0</v>
       </c>
       <c r="F60" s="2" t="n">
         <v>0.0</v>
@@ -1981,26 +1981,26 @@
     <row r="61">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>Optoelectronics</t>
+          <t>Resistors</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
         <is>
-          <t>LTST-C193KFKT-5A</t>
+          <t>RC0402FR-0731K6L</t>
         </is>
       </c>
       <c r="C61" s="2" t="inlineStr">
         <is>
-          <t>0603</t>
+          <t>0402</t>
         </is>
       </c>
       <c r="D61" s="2" t="inlineStr">
         <is>
-          <t>C284922</t>
+          <t>C276265</t>
         </is>
       </c>
       <c r="E61" s="2" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="F61" s="2" t="n">
         <v>0.0</v>
@@ -2012,26 +2012,26 @@
     <row r="62">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>Power Management (PMIC)</t>
+          <t>Inductors, Coils, Chokes</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
         <is>
-          <t>LM5163DDAR</t>
+          <t>G48C01S</t>
         </is>
       </c>
       <c r="C62" s="2" t="inlineStr">
         <is>
-          <t>ESOP-8</t>
+          <t>SMD</t>
         </is>
       </c>
       <c r="D62" s="2" t="inlineStr">
         <is>
-          <t>C2873264</t>
+          <t>C2827284</t>
         </is>
       </c>
       <c r="E62" s="2" t="n">
-        <v>0.0</v>
+        <v>280.0</v>
       </c>
       <c r="F62" s="2" t="n">
         <v>0.0</v>
@@ -2043,26 +2043,26 @@
     <row r="63">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>Connectors</t>
+          <t>Diodes</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
         <is>
-          <t>PM254-2-12-W-8.5</t>
+          <t>LMSZ5265BT1G</t>
         </is>
       </c>
       <c r="C63" s="2" t="inlineStr">
         <is>
-          <t>Push-Pull,P=2.54mm</t>
+          <t>SOD-123</t>
         </is>
       </c>
       <c r="D63" s="2" t="inlineStr">
         <is>
-          <t>C2897432</t>
+          <t>C2847461</t>
         </is>
       </c>
       <c r="E63" s="2" t="n">
-        <v>100.0</v>
+        <v>272.0</v>
       </c>
       <c r="F63" s="2" t="n">
         <v>0.0</v>
@@ -2074,26 +2074,26 @@
     <row r="64">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>Switches</t>
+          <t>Optoelectronics</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
         <is>
-          <t>CFS-0400TB</t>
+          <t>LTST-C193KFKT-5A</t>
         </is>
       </c>
       <c r="C64" s="2" t="inlineStr">
         <is>
-          <t>SMD</t>
+          <t>0603</t>
         </is>
       </c>
       <c r="D64" s="2" t="inlineStr">
         <is>
-          <t>C2921584</t>
+          <t>C284922</t>
         </is>
       </c>
       <c r="E64" s="2" t="n">
-        <v>60.0</v>
+        <v>50.0</v>
       </c>
       <c r="F64" s="2" t="n">
         <v>0.0</v>
@@ -2105,26 +2105,26 @@
     <row r="65">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>Resistors</t>
+          <t>Power Management (PMIC)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
         <is>
-          <t>RC0201FR-0715KL</t>
+          <t>LM5163DDAR</t>
         </is>
       </c>
       <c r="C65" s="2" t="inlineStr">
         <is>
-          <t>0201</t>
+          <t>ESOP-8</t>
         </is>
       </c>
       <c r="D65" s="2" t="inlineStr">
         <is>
-          <t>C295774</t>
+          <t>C2873264</t>
         </is>
       </c>
       <c r="E65" s="2" t="n">
-        <v>10000.0</v>
+        <v>0.0</v>
       </c>
       <c r="F65" s="2" t="n">
         <v>0.0</v>
@@ -2136,26 +2136,26 @@
     <row r="66">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>Filters</t>
+          <t>Connectors</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
         <is>
-          <t>CND-WCM0805M801-2</t>
+          <t>PM254-2-12-W-8.5</t>
         </is>
       </c>
       <c r="C66" s="2" t="inlineStr">
         <is>
-          <t>0805</t>
+          <t>Push-Pull,P=2.54mm</t>
         </is>
       </c>
       <c r="D66" s="2" t="inlineStr">
         <is>
-          <t>C3020807</t>
+          <t>C2897432</t>
         </is>
       </c>
       <c r="E66" s="2" t="n">
-        <v>600.0</v>
+        <v>100.0</v>
       </c>
       <c r="F66" s="2" t="n">
         <v>0.0</v>
@@ -2167,26 +2167,26 @@
     <row r="67">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>Capacitors</t>
+          <t>Switches</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
         <is>
-          <t>0805B102K102CT</t>
+          <t>CFS-0400TB</t>
         </is>
       </c>
       <c r="C67" s="2" t="inlineStr">
         <is>
-          <t>0805</t>
+          <t>SMD</t>
         </is>
       </c>
       <c r="D67" s="2" t="inlineStr">
         <is>
-          <t>C303890</t>
+          <t>C2921584</t>
         </is>
       </c>
       <c r="E67" s="2" t="n">
-        <v>100.0</v>
+        <v>60.0</v>
       </c>
       <c r="F67" s="2" t="n">
         <v>0.0</v>
@@ -2198,26 +2198,26 @@
     <row r="68">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>Capacitors</t>
+          <t>Resistors</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
         <is>
-          <t>CL05B105KQ5NQNC</t>
+          <t>RC0201FR-0715KL</t>
         </is>
       </c>
       <c r="C68" s="2" t="inlineStr">
         <is>
-          <t>0402</t>
+          <t>0201</t>
         </is>
       </c>
       <c r="D68" s="2" t="inlineStr">
         <is>
-          <t>C307427</t>
+          <t>C295774</t>
         </is>
       </c>
       <c r="E68" s="2" t="n">
-        <v>1000.0</v>
+        <v>10000.0</v>
       </c>
       <c r="F68" s="2" t="n">
         <v>0.0</v>
@@ -2229,26 +2229,26 @@
     <row r="69">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>Capacitors</t>
+          <t>Filters</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
         <is>
-          <t>CL05A106MP5NUNC</t>
+          <t>CND-WCM0805M801-2</t>
         </is>
       </c>
       <c r="C69" s="2" t="inlineStr">
         <is>
-          <t>0402</t>
+          <t>0805</t>
         </is>
       </c>
       <c r="D69" s="2" t="inlineStr">
         <is>
-          <t>C315248</t>
+          <t>C3020807</t>
         </is>
       </c>
       <c r="E69" s="2" t="n">
-        <v>1000.0</v>
+        <v>600.0</v>
       </c>
       <c r="F69" s="2" t="n">
         <v>0.0</v>
@@ -2260,26 +2260,26 @@
     <row r="70">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>Connectors</t>
+          <t>Capacitors</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
         <is>
-          <t>894-70-048-10-001101</t>
+          <t>0805B102K102CT</t>
         </is>
       </c>
       <c r="C70" s="2" t="inlineStr">
         <is>
-          <t>Plugin,P=2.54mm</t>
+          <t>0805</t>
         </is>
       </c>
       <c r="D70" s="2" t="inlineStr">
         <is>
-          <t>C3325244</t>
+          <t>C303890</t>
         </is>
       </c>
       <c r="E70" s="2" t="n">
-        <v>0.0</v>
+        <v>100.0</v>
       </c>
       <c r="F70" s="2" t="n">
         <v>0.0</v>
@@ -2291,26 +2291,26 @@
     <row r="71">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>Connectors</t>
+          <t>Capacitors</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
         <is>
-          <t>HTSW-103-07-T-T</t>
+          <t>CL05B105KQ5NQNC</t>
         </is>
       </c>
       <c r="C71" s="2" t="inlineStr">
         <is>
-          <t>Plugin,P=2.54mm</t>
+          <t>0402</t>
         </is>
       </c>
       <c r="D71" s="2" t="inlineStr">
         <is>
-          <t>C3330089</t>
+          <t>C307427</t>
         </is>
       </c>
       <c r="E71" s="2" t="n">
-        <v>0.0</v>
+        <v>1000.0</v>
       </c>
       <c r="F71" s="2" t="n">
         <v>0.0</v>
@@ -2322,29 +2322,29 @@
     <row r="72">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>Connectors</t>
+          <t>Capacitors</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
         <is>
-          <t>M20-9990345</t>
+          <t>CL05A106MP5NUNC</t>
         </is>
       </c>
       <c r="C72" s="2" t="inlineStr">
         <is>
-          <t>Plugin,P=2.54mm</t>
+          <t>0402</t>
         </is>
       </c>
       <c r="D72" s="2" t="inlineStr">
         <is>
-          <t>C3337081</t>
+          <t>C315248</t>
         </is>
       </c>
       <c r="E72" s="2" t="n">
-        <v>0.0</v>
+        <v>1000.0</v>
       </c>
       <c r="F72" s="2" t="n">
-        <v>2007.0</v>
+        <v>0.0</v>
       </c>
       <c r="G72" s="2" t="n">
         <v>0.0</v>
@@ -2353,26 +2353,26 @@
     <row r="73">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>Capacitors</t>
+          <t>Connectors</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
         <is>
-          <t>GRM033R61C105ME15D</t>
+          <t>894-70-048-10-001101</t>
         </is>
       </c>
       <c r="C73" s="2" t="inlineStr">
         <is>
-          <t>0201</t>
+          <t>Plugin,P=2.54mm</t>
         </is>
       </c>
       <c r="D73" s="2" t="inlineStr">
         <is>
-          <t>C335102</t>
+          <t>C3325244</t>
         </is>
       </c>
       <c r="E73" s="2" t="n">
-        <v>1000.0</v>
+        <v>0.0</v>
       </c>
       <c r="F73" s="2" t="n">
         <v>0.0</v>
@@ -2384,26 +2384,26 @@
     <row r="74">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>Resistors</t>
+          <t>Connectors</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
         <is>
-          <t>RC0201FR-0745K3L</t>
+          <t>HTSW-103-07-T-T</t>
         </is>
       </c>
       <c r="C74" s="2" t="inlineStr">
         <is>
-          <t>0201</t>
+          <t>Plugin,P=2.54mm</t>
         </is>
       </c>
       <c r="D74" s="2" t="inlineStr">
         <is>
-          <t>C364365</t>
+          <t>C3330089</t>
         </is>
       </c>
       <c r="E74" s="2" t="n">
-        <v>578.0</v>
+        <v>0.0</v>
       </c>
       <c r="F74" s="2" t="n">
         <v>0.0</v>
@@ -2415,29 +2415,29 @@
     <row r="75">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>Capacitors</t>
+          <t>Connectors</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
         <is>
-          <t>GRM0335C1H471JE01D</t>
+          <t>M20-9990345</t>
         </is>
       </c>
       <c r="C75" s="2" t="inlineStr">
         <is>
-          <t>0201</t>
+          <t>Plugin,P=2.54mm</t>
         </is>
       </c>
       <c r="D75" s="2" t="inlineStr">
         <is>
-          <t>C3886751</t>
+          <t>C3337081</t>
         </is>
       </c>
       <c r="E75" s="2" t="n">
-        <v>1000.0</v>
+        <v>0.0</v>
       </c>
       <c r="F75" s="2" t="n">
-        <v>0.0</v>
+        <v>2007.0</v>
       </c>
       <c r="G75" s="2" t="n">
         <v>0.0</v>
@@ -2446,29 +2446,29 @@
     <row r="76">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>Magnetic Sensors</t>
+          <t>Capacitors</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
         <is>
-          <t>MMC5983MA</t>
+          <t>GRM033R61C105ME15D</t>
         </is>
       </c>
       <c r="C76" s="2" t="inlineStr">
         <is>
-          <t>LGA-16(3x3)</t>
+          <t>0201</t>
         </is>
       </c>
       <c r="D76" s="2" t="inlineStr">
         <is>
-          <t>C404329</t>
+          <t>C335102</t>
         </is>
       </c>
       <c r="E76" s="2" t="n">
-        <v>0.0</v>
+        <v>1000.0</v>
       </c>
       <c r="F76" s="2" t="n">
-        <v>500.0</v>
+        <v>0.0</v>
       </c>
       <c r="G76" s="2" t="n">
         <v>0.0</v>
@@ -2477,26 +2477,26 @@
     <row r="77">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>Inductors, Coils, Chokes</t>
+          <t>Resistors</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
         <is>
-          <t>VLS6045EX-101M</t>
+          <t>RC0201FR-0745K3L</t>
         </is>
       </c>
       <c r="C77" s="2" t="inlineStr">
         <is>
-          <t>SMD,6x6mm</t>
+          <t>0201</t>
         </is>
       </c>
       <c r="D77" s="2" t="inlineStr">
         <is>
-          <t>C404507</t>
+          <t>C364365</t>
         </is>
       </c>
       <c r="E77" s="2" t="n">
-        <v>0.0</v>
+        <v>578.0</v>
       </c>
       <c r="F77" s="2" t="n">
         <v>0.0</v>
@@ -2508,12 +2508,12 @@
     <row r="78">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>Resistors</t>
+          <t>Capacitors</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
         <is>
-          <t>0201WMF1212TEE</t>
+          <t>GRM0335C1H471JE01D</t>
         </is>
       </c>
       <c r="C78" s="2" t="inlineStr">
@@ -2523,11 +2523,11 @@
       </c>
       <c r="D78" s="2" t="inlineStr">
         <is>
-          <t>C423764</t>
+          <t>C3886751</t>
         </is>
       </c>
       <c r="E78" s="2" t="n">
-        <v>15452.0</v>
+        <v>1000.0</v>
       </c>
       <c r="F78" s="2" t="n">
         <v>0.0</v>
@@ -2539,29 +2539,29 @@
     <row r="79">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>Circuit Protection</t>
+          <t>Magnetic Sensors</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
         <is>
-          <t>SMAJ54CA</t>
+          <t>MMC5983MA</t>
         </is>
       </c>
       <c r="C79" s="2" t="inlineStr">
         <is>
-          <t>SMA</t>
+          <t>LGA-16(3x3)</t>
         </is>
       </c>
       <c r="D79" s="2" t="inlineStr">
         <is>
-          <t>C435567</t>
+          <t>C404329</t>
         </is>
       </c>
       <c r="E79" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F79" s="2" t="n">
-        <v>0.0</v>
+        <v>500.0</v>
       </c>
       <c r="G79" s="2" t="n">
         <v>0.0</v>
@@ -2575,7 +2575,7 @@
       </c>
       <c r="B80" s="2" t="inlineStr">
         <is>
-          <t>PSPNAQ6045-100M</t>
+          <t>VLS6045EX-101M</t>
         </is>
       </c>
       <c r="C80" s="2" t="inlineStr">
@@ -2585,7 +2585,7 @@
       </c>
       <c r="D80" s="2" t="inlineStr">
         <is>
-          <t>C436755</t>
+          <t>C404507</t>
         </is>
       </c>
       <c r="E80" s="2" t="n">
@@ -2601,26 +2601,26 @@
     <row r="81">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>Diodes</t>
+          <t>Resistors</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
         <is>
-          <t>MM1Z62B</t>
+          <t>0201WMF1212TEE</t>
         </is>
       </c>
       <c r="C81" s="2" t="inlineStr">
         <is>
-          <t>SOD-123</t>
+          <t>0201</t>
         </is>
       </c>
       <c r="D81" s="2" t="inlineStr">
         <is>
-          <t>C438324</t>
+          <t>C423764</t>
         </is>
       </c>
       <c r="E81" s="2" t="n">
-        <v>142.0</v>
+        <v>15452.0</v>
       </c>
       <c r="F81" s="2" t="n">
         <v>0.0</v>
@@ -2632,29 +2632,29 @@
     <row r="82">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>Data Acquisition</t>
+          <t>Circuit Protection</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
         <is>
-          <t>ADS1115IDGST</t>
+          <t>SMAJ54CA</t>
         </is>
       </c>
       <c r="C82" s="2" t="inlineStr">
         <is>
-          <t>VSSOP-10-0.5mm</t>
+          <t>SMA</t>
         </is>
       </c>
       <c r="D82" s="2" t="inlineStr">
         <is>
-          <t>C468683</t>
+          <t>C435567</t>
         </is>
       </c>
       <c r="E82" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F82" s="2" t="n">
-        <v>500.0</v>
+        <v>0.0</v>
       </c>
       <c r="G82" s="2" t="n">
         <v>0.0</v>
@@ -2663,26 +2663,26 @@
     <row r="83">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>Power Management (PMIC)</t>
+          <t>Inductors, Coils, Chokes</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
         <is>
-          <t>LM5160ADNTR</t>
+          <t>PSPNAQ6045-100M</t>
         </is>
       </c>
       <c r="C83" s="2" t="inlineStr">
         <is>
-          <t>WSON-12-EP(4x4)</t>
+          <t>SMD,6x6mm</t>
         </is>
       </c>
       <c r="D83" s="2" t="inlineStr">
         <is>
-          <t>C473375</t>
+          <t>C436755</t>
         </is>
       </c>
       <c r="E83" s="2" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="F83" s="2" t="n">
         <v>0.0</v>
@@ -2694,26 +2694,26 @@
     <row r="84">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>Connectors</t>
+          <t>Diodes</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
         <is>
-          <t>PZ254-2-12-WS</t>
+          <t>MM1Z62B</t>
         </is>
       </c>
       <c r="C84" s="2" t="inlineStr">
         <is>
-          <t>SMD,P=2.54mm</t>
+          <t>SOD-123</t>
         </is>
       </c>
       <c r="D84" s="2" t="inlineStr">
         <is>
-          <t>C5149362</t>
+          <t>C438324</t>
         </is>
       </c>
       <c r="E84" s="2" t="n">
-        <v>100.0</v>
+        <v>9.0</v>
       </c>
       <c r="F84" s="2" t="n">
         <v>0.0</v>
@@ -2725,29 +2725,29 @@
     <row r="85">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>Interface</t>
+          <t>Data Acquisition</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
         <is>
-          <t>RTL8305NB-CG</t>
+          <t>ADS1115IDGST</t>
         </is>
       </c>
       <c r="C85" s="2" t="inlineStr">
         <is>
-          <t>QFN-48-EP(6x6)</t>
+          <t>VSSOP-10-0.5mm</t>
         </is>
       </c>
       <c r="D85" s="2" t="inlineStr">
         <is>
-          <t>C52146</t>
+          <t>C468683</t>
         </is>
       </c>
       <c r="E85" s="2" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="F85" s="2" t="n">
-        <v>0.0</v>
+        <v>500.0</v>
       </c>
       <c r="G85" s="2" t="n">
         <v>0.0</v>
@@ -2756,26 +2756,26 @@
     <row r="86">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>Transistors/Thyristors</t>
+          <t>Power Management (PMIC)</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
         <is>
-          <t>WST06P06</t>
+          <t>LM5160ADNTR</t>
         </is>
       </c>
       <c r="C86" s="2" t="inlineStr">
         <is>
-          <t>SOT-23-3L</t>
+          <t>WSON-12-EP(4x4)</t>
         </is>
       </c>
       <c r="D86" s="2" t="inlineStr">
         <is>
-          <t>C5242059</t>
+          <t>C473375</t>
         </is>
       </c>
       <c r="E86" s="2" t="n">
-        <v>90.0</v>
+        <v>100.0</v>
       </c>
       <c r="F86" s="2" t="n">
         <v>0.0</v>
@@ -2787,26 +2787,26 @@
     <row r="87">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>Power Management (PMIC)</t>
+          <t>Connectors</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
         <is>
-          <t>AP7370-33Y-13</t>
+          <t>PZ254-2-12-WS</t>
         </is>
       </c>
       <c r="C87" s="2" t="inlineStr">
         <is>
-          <t>SOT-89-3</t>
+          <t>SMD,P=2.54mm</t>
         </is>
       </c>
       <c r="D87" s="2" t="inlineStr">
         <is>
-          <t>C5329418</t>
+          <t>C5149362</t>
         </is>
       </c>
       <c r="E87" s="2" t="n">
-        <v>0.0</v>
+        <v>100.0</v>
       </c>
       <c r="F87" s="2" t="n">
         <v>0.0</v>
@@ -2818,26 +2818,26 @@
     <row r="88">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>Capacitors</t>
+          <t>Interface</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
         <is>
-          <t>GRM32EC72A106KE05L</t>
+          <t>RTL8305NB-CG</t>
         </is>
       </c>
       <c r="C88" s="2" t="inlineStr">
         <is>
-          <t>1210</t>
+          <t>QFN-48-EP(6x6)</t>
         </is>
       </c>
       <c r="D88" s="2" t="inlineStr">
         <is>
-          <t>C576517</t>
+          <t>C52146</t>
         </is>
       </c>
       <c r="E88" s="2" t="n">
-        <v>200.0</v>
+        <v>5.0</v>
       </c>
       <c r="F88" s="2" t="n">
         <v>0.0</v>
@@ -2849,26 +2849,26 @@
     <row r="89">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>Capacitors</t>
+          <t>Transistors/Thyristors</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
         <is>
-          <t>CC0402KRX7R9BB103</t>
+          <t>WST06P06</t>
         </is>
       </c>
       <c r="C89" s="2" t="inlineStr">
         <is>
-          <t>0402</t>
+          <t>SOT-23-3L</t>
         </is>
       </c>
       <c r="D89" s="2" t="inlineStr">
         <is>
-          <t>C60133</t>
+          <t>C5242059</t>
         </is>
       </c>
       <c r="E89" s="2" t="n">
-        <v>5000.0</v>
+        <v>90.0</v>
       </c>
       <c r="F89" s="2" t="n">
         <v>0.0</v>
@@ -2880,26 +2880,26 @@
     <row r="90">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>Resistors</t>
+          <t>Connectors</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
         <is>
-          <t>RC0402FR-072KL</t>
+          <t>RH-5000</t>
         </is>
       </c>
       <c r="C90" s="2" t="inlineStr">
         <is>
-          <t>0402</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D90" s="2" t="inlineStr">
         <is>
-          <t>C60488</t>
+          <t>C5277086</t>
         </is>
       </c>
       <c r="E90" s="2" t="n">
-        <v>0.0</v>
+        <v>100.0</v>
       </c>
       <c r="F90" s="2" t="n">
         <v>0.0</v>
@@ -2911,22 +2911,22 @@
     <row r="91">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>Crystals, Oscillators, Resonators</t>
+          <t>Power Management (PMIC)</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
         <is>
-          <t>X322525MQB4SI</t>
+          <t>AP7370-33Y-13</t>
         </is>
       </c>
       <c r="C91" s="2" t="inlineStr">
         <is>
-          <t>SMD3225-4P</t>
+          <t>SOT-89-3</t>
         </is>
       </c>
       <c r="D91" s="2" t="inlineStr">
         <is>
-          <t>C70585</t>
+          <t>C5329418</t>
         </is>
       </c>
       <c r="E91" s="2" t="n">
@@ -2942,26 +2942,26 @@
     <row r="92">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>Connectors</t>
+          <t>Capacitors</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
         <is>
-          <t>RC01812</t>
+          <t>GRM32EC72A106KE05L</t>
         </is>
       </c>
       <c r="C92" s="2" t="inlineStr">
         <is>
-          <t>SMD</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="D92" s="2" t="inlineStr">
         <is>
-          <t>C708645</t>
+          <t>C576517</t>
         </is>
       </c>
       <c r="E92" s="2" t="n">
-        <v>100.0</v>
+        <v>75.0</v>
       </c>
       <c r="F92" s="2" t="n">
         <v>0.0</v>
@@ -2973,26 +2973,26 @@
     <row r="93">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>Switches</t>
+          <t>Capacitors</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
         <is>
-          <t>TS-1088-AR02016</t>
+          <t>CC0402KRX7R9BB103</t>
         </is>
       </c>
       <c r="C93" s="2" t="inlineStr">
         <is>
-          <t>SMD</t>
+          <t>0402</t>
         </is>
       </c>
       <c r="D93" s="2" t="inlineStr">
         <is>
-          <t>C720477</t>
+          <t>C60133</t>
         </is>
       </c>
       <c r="E93" s="2" t="n">
-        <v>100.0</v>
+        <v>5000.0</v>
       </c>
       <c r="F93" s="2" t="n">
         <v>0.0</v>
@@ -3004,26 +3004,26 @@
     <row r="94">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>Inductors, Coils, Chokes</t>
+          <t>Resistors</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
         <is>
-          <t>GA030G00</t>
+          <t>RC0402FR-072KL</t>
         </is>
       </c>
       <c r="C94" s="2" t="inlineStr">
         <is>
-          <t>SMD-6P,4.6x3.4mm</t>
+          <t>0402</t>
         </is>
       </c>
       <c r="D94" s="2" t="inlineStr">
         <is>
-          <t>C7501940</t>
+          <t>C60488</t>
         </is>
       </c>
       <c r="E94" s="2" t="n">
-        <v>600.0</v>
+        <v>0.0</v>
       </c>
       <c r="F94" s="2" t="n">
         <v>0.0</v>
@@ -3035,22 +3035,22 @@
     <row r="95">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>Capacitors</t>
+          <t>Crystals, Oscillators, Resonators</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
         <is>
-          <t>GRM0335C1H3R9CA01D</t>
+          <t>X322525MQB4SI</t>
         </is>
       </c>
       <c r="C95" s="2" t="inlineStr">
         <is>
-          <t>0201</t>
+          <t>SMD3225-4P</t>
         </is>
       </c>
       <c r="D95" s="2" t="inlineStr">
         <is>
-          <t>C76926</t>
+          <t>C70585</t>
         </is>
       </c>
       <c r="E95" s="2" t="n">
@@ -3066,26 +3066,26 @@
     <row r="96">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>Crystals, Oscillators, Resonators</t>
+          <t>Connectors</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
         <is>
-          <t>NX2016SA-25MHZ-STD-CZS-2</t>
+          <t>RC01812</t>
         </is>
       </c>
       <c r="C96" s="2" t="inlineStr">
         <is>
-          <t>SMD2016-4P</t>
+          <t>SMD</t>
         </is>
       </c>
       <c r="D96" s="2" t="inlineStr">
         <is>
-          <t>C843258</t>
+          <t>C708645</t>
         </is>
       </c>
       <c r="E96" s="2" t="n">
-        <v>150.0</v>
+        <v>100.0</v>
       </c>
       <c r="F96" s="2" t="n">
         <v>0.0</v>
@@ -3097,26 +3097,26 @@
     <row r="97">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>Resistors</t>
+          <t>Switches</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
         <is>
-          <t>RC0201DR-0749K9L</t>
+          <t>TS-1088-AR02016</t>
         </is>
       </c>
       <c r="C97" s="2" t="inlineStr">
         <is>
-          <t>0201</t>
+          <t>SMD</t>
         </is>
       </c>
       <c r="D97" s="2" t="inlineStr">
         <is>
-          <t>C851750</t>
+          <t>C720477</t>
         </is>
       </c>
       <c r="E97" s="2" t="n">
-        <v>3940.0</v>
+        <v>100.0</v>
       </c>
       <c r="F97" s="2" t="n">
         <v>0.0</v>
@@ -3128,26 +3128,26 @@
     <row r="98">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>Connectors</t>
+          <t>Inductors, Coils, Chokes</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
         <is>
-          <t>DS1129-04-S8B0P-X</t>
+          <t>GA030G00</t>
         </is>
       </c>
       <c r="C98" s="2" t="inlineStr">
         <is>
-          <t>Plugin</t>
+          <t>SMD-6P,4.6x3.4mm</t>
         </is>
       </c>
       <c r="D98" s="2" t="inlineStr">
         <is>
-          <t>C86581</t>
+          <t>C7501940</t>
         </is>
       </c>
       <c r="E98" s="2" t="n">
-        <v>475.0</v>
+        <v>600.0</v>
       </c>
       <c r="F98" s="2" t="n">
         <v>0.0</v>
@@ -3159,26 +3159,26 @@
     <row r="99">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>Resistors</t>
+          <t>Capacitors</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
         <is>
-          <t>RC0402FR-0749R9L</t>
+          <t>GRM0335C1H3R9CA01D</t>
         </is>
       </c>
       <c r="C99" s="2" t="inlineStr">
         <is>
-          <t>0402</t>
+          <t>0201</t>
         </is>
       </c>
       <c r="D99" s="2" t="inlineStr">
         <is>
-          <t>C87044</t>
+          <t>C76926</t>
         </is>
       </c>
       <c r="E99" s="2" t="n">
-        <v>90.0</v>
+        <v>0.0</v>
       </c>
       <c r="F99" s="2" t="n">
         <v>0.0</v>
@@ -3190,26 +3190,26 @@
     <row r="100">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>Diodes</t>
+          <t>Crystals, Oscillators, Resonators</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
         <is>
-          <t>SZMM3Z10VT1G</t>
+          <t>NX2016SA-25MHZ-STD-CZS-2</t>
         </is>
       </c>
       <c r="C100" s="2" t="inlineStr">
         <is>
-          <t>SOD-323</t>
+          <t>SMD2016-4P</t>
         </is>
       </c>
       <c r="D100" s="2" t="inlineStr">
         <is>
-          <t>C894520</t>
+          <t>C843258</t>
         </is>
       </c>
       <c r="E100" s="2" t="n">
-        <v>50.0</v>
+        <v>150.0</v>
       </c>
       <c r="F100" s="2" t="n">
         <v>0.0</v>
@@ -3221,26 +3221,26 @@
     <row r="101">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>Filters</t>
+          <t>Resistors</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
         <is>
-          <t>ACM2520-601-2P-T002</t>
+          <t>RC0201DR-0749K9L</t>
         </is>
       </c>
       <c r="C101" s="2" t="inlineStr">
         <is>
-          <t>SMD</t>
+          <t>0201</t>
         </is>
       </c>
       <c r="D101" s="2" t="inlineStr">
         <is>
-          <t>C92013</t>
+          <t>C851750</t>
         </is>
       </c>
       <c r="E101" s="2" t="n">
-        <v>50.0</v>
+        <v>3940.0</v>
       </c>
       <c r="F101" s="2" t="n">
         <v>0.0</v>
@@ -3252,29 +3252,29 @@
     <row r="102">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>Optoelectronics</t>
+          <t>Resistors</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
         <is>
-          <t>LTST-S270TBKT</t>
+          <t>RC0201DR-07681RL</t>
         </is>
       </c>
       <c r="C102" s="2" t="inlineStr">
         <is>
-          <t>SMD,1.2x1.6mm</t>
+          <t>0201</t>
         </is>
       </c>
       <c r="D102" s="2" t="inlineStr">
         <is>
-          <t>C125115</t>
+          <t>C851780</t>
         </is>
       </c>
       <c r="E102" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F102" s="2" t="n">
-        <v>1100.0</v>
+        <v>0.0</v>
       </c>
       <c r="G102" s="2" t="n">
         <v>0.0</v>
@@ -3283,12 +3283,12 @@
     <row r="103">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>Resistors</t>
+          <t>Capacitors</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
         <is>
-          <t>RC0402FR-074K99L</t>
+          <t>GCM155R71H104KE02D</t>
         </is>
       </c>
       <c r="C103" s="2" t="inlineStr">
@@ -3298,14 +3298,14 @@
       </c>
       <c r="D103" s="2" t="inlineStr">
         <is>
-          <t>C137965</t>
+          <t>C85858</t>
         </is>
       </c>
       <c r="E103" s="2" t="n">
-        <v>0.0</v>
+        <v>10000.0</v>
       </c>
       <c r="F103" s="2" t="n">
-        <v>1100.0</v>
+        <v>0.0</v>
       </c>
       <c r="G103" s="2" t="n">
         <v>0.0</v>
@@ -3314,29 +3314,29 @@
     <row r="104">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>Resistors</t>
+          <t>Connectors</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
         <is>
-          <t>RC0402FR-0749K9L</t>
+          <t>DS1129-04-S8B0P-X</t>
         </is>
       </c>
       <c r="C104" s="2" t="inlineStr">
         <is>
-          <t>0402</t>
+          <t>Plugin</t>
         </is>
       </c>
       <c r="D104" s="2" t="inlineStr">
         <is>
-          <t>C137969</t>
+          <t>C86581</t>
         </is>
       </c>
       <c r="E104" s="2" t="n">
-        <v>0.0</v>
+        <v>350.0</v>
       </c>
       <c r="F104" s="2" t="n">
-        <v>9980.0</v>
+        <v>0.0</v>
       </c>
       <c r="G104" s="2" t="n">
         <v>0.0</v>
@@ -3350,24 +3350,24 @@
       </c>
       <c r="B105" s="2" t="inlineStr">
         <is>
-          <t>RC0201FR-073KL</t>
+          <t>RC0402FR-0749R9L</t>
         </is>
       </c>
       <c r="C105" s="2" t="inlineStr">
         <is>
-          <t>0201</t>
+          <t>0402</t>
         </is>
       </c>
       <c r="D105" s="2" t="inlineStr">
         <is>
-          <t>C142016</t>
+          <t>C87044</t>
         </is>
       </c>
       <c r="E105" s="2" t="n">
-        <v>0.0</v>
+        <v>90.0</v>
       </c>
       <c r="F105" s="2" t="n">
-        <v>60.0</v>
+        <v>0.0</v>
       </c>
       <c r="G105" s="2" t="n">
         <v>0.0</v>
@@ -3376,29 +3376,29 @@
     <row r="106">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>Interface</t>
+          <t>Diodes</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
         <is>
-          <t>88LX5153A0-BUU2C000</t>
+          <t>SZMM3Z10VT1G</t>
         </is>
       </c>
       <c r="C106" s="2" t="inlineStr">
         <is>
-          <t>BGA-186(10x10)</t>
+          <t>SOD-323</t>
         </is>
       </c>
       <c r="D106" s="2" t="inlineStr">
         <is>
-          <t>C1550519</t>
+          <t>C894520</t>
         </is>
       </c>
       <c r="E106" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F106" s="2" t="n">
-        <v>20.0</v>
+        <v>0.0</v>
       </c>
       <c r="G106" s="2" t="n">
         <v>0.0</v>
@@ -3407,29 +3407,29 @@
     <row r="107">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>Resistors</t>
+          <t>Filters</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
         <is>
-          <t>RC0201FR-075K9L</t>
+          <t>ACM2520-601-2P-T002</t>
         </is>
       </c>
       <c r="C107" s="2" t="inlineStr">
         <is>
-          <t>0201</t>
+          <t>SMD</t>
         </is>
       </c>
       <c r="D107" s="2" t="inlineStr">
         <is>
-          <t>C155740</t>
+          <t>C92013</t>
         </is>
       </c>
       <c r="E107" s="2" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="F107" s="2" t="n">
-        <v>30.0</v>
+        <v>0.0</v>
       </c>
       <c r="G107" s="2" t="n">
         <v>0.0</v>
@@ -3438,29 +3438,29 @@
     <row r="108">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>Global Sourcing Parts</t>
+          <t>Optoelectronics</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
         <is>
-          <t>831056295</t>
+          <t>LTST-S270TBKT</t>
         </is>
       </c>
       <c r="C108" s="2" t="inlineStr">
         <is>
-          <t>SMD2520-4P</t>
+          <t>SMD,1.2x1.6mm</t>
         </is>
       </c>
       <c r="D108" s="2" t="inlineStr">
         <is>
-          <t>C17219465</t>
+          <t>C125115</t>
         </is>
       </c>
       <c r="E108" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F108" s="2" t="n">
-        <v>500.0</v>
+        <v>1100.0</v>
       </c>
       <c r="G108" s="2" t="n">
         <v>0.0</v>
@@ -3469,29 +3469,29 @@
     <row r="109">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>Connectors</t>
+          <t>Resistors</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
         <is>
-          <t>BM06B-GHS-TBT(LF)(SN)</t>
+          <t>RC0402FR-074K99L</t>
         </is>
       </c>
       <c r="C109" s="2" t="inlineStr">
         <is>
-          <t>SMD,P=1.25mm</t>
+          <t>0402</t>
         </is>
       </c>
       <c r="D109" s="2" t="inlineStr">
         <is>
-          <t>C189892</t>
+          <t>C137965</t>
         </is>
       </c>
       <c r="E109" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F109" s="2" t="n">
-        <v>5000.0</v>
+        <v>1100.0</v>
       </c>
       <c r="G109" s="2" t="n">
         <v>0.0</v>
@@ -3500,29 +3500,29 @@
     <row r="110">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>Inductors, Coils, Chokes</t>
+          <t>Resistors</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
         <is>
-          <t>SRP1050WA-220M</t>
+          <t>RC0402FR-0749K9L</t>
         </is>
       </c>
       <c r="C110" s="2" t="inlineStr">
         <is>
-          <t>SMD,11x10mm</t>
+          <t>0402</t>
         </is>
       </c>
       <c r="D110" s="2" t="inlineStr">
         <is>
-          <t>C19947668</t>
+          <t>C137969</t>
         </is>
       </c>
       <c r="E110" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F110" s="2" t="n">
-        <v>30.0</v>
+        <v>9980.0</v>
       </c>
       <c r="G110" s="2" t="n">
         <v>0.0</v>
@@ -3531,29 +3531,29 @@
     <row r="111">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>Global Sourcing Parts</t>
+          <t>Resistors</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
         <is>
-          <t>SRP7050WA-100M</t>
+          <t>RC0201FR-073KL</t>
         </is>
       </c>
       <c r="C111" s="2" t="inlineStr">
         <is>
-          <t>SMD,7.9x7.3mm</t>
+          <t>0201</t>
         </is>
       </c>
       <c r="D111" s="2" t="inlineStr">
         <is>
-          <t>C19947697</t>
+          <t>C142016</t>
         </is>
       </c>
       <c r="E111" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F111" s="2" t="n">
-        <v>90.0</v>
+        <v>60.0</v>
       </c>
       <c r="G111" s="2" t="n">
         <v>0.0</v>
@@ -3562,29 +3562,29 @@
     <row r="112">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>Capacitors</t>
+          <t>Interface</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
         <is>
-          <t>GRM155D71A475ME15J</t>
+          <t>88LX5153A0-BUU2C000</t>
         </is>
       </c>
       <c r="C112" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>BGA-186(10x10)</t>
         </is>
       </c>
       <c r="D112" s="2" t="inlineStr">
         <is>
-          <t>C20044523</t>
+          <t>C1550519</t>
         </is>
       </c>
       <c r="E112" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F112" s="2" t="n">
-        <v>30.0</v>
+        <v>20.0</v>
       </c>
       <c r="G112" s="2" t="n">
         <v>0.0</v>
@@ -3593,29 +3593,29 @@
     <row r="113">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>Connectors</t>
+          <t>Resistors</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
         <is>
-          <t>BM06B-GHS-TBT</t>
+          <t>RC0201FR-075K9L</t>
         </is>
       </c>
       <c r="C113" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0201</t>
         </is>
       </c>
       <c r="D113" s="2" t="inlineStr">
         <is>
-          <t>C20089153</t>
+          <t>C155740</t>
         </is>
       </c>
       <c r="E113" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F113" s="2" t="n">
-        <v>20.0</v>
+        <v>30.0</v>
       </c>
       <c r="G113" s="2" t="n">
         <v>0.0</v>
@@ -3624,29 +3624,29 @@
     <row r="114">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>Motor Driver ICs</t>
+          <t>Global Sourcing Parts</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
         <is>
-          <t>DRV8849RHHR</t>
+          <t>831056295</t>
         </is>
       </c>
       <c r="C114" s="2" t="inlineStr">
         <is>
-          <t>VQFN-36(6x6)</t>
+          <t>SMD2520-4P</t>
         </is>
       </c>
       <c r="D114" s="2" t="inlineStr">
         <is>
-          <t>C20345377</t>
+          <t>C17219465</t>
         </is>
       </c>
       <c r="E114" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F114" s="2" t="n">
-        <v>90.0</v>
+        <v>500.0</v>
       </c>
       <c r="G114" s="2" t="n">
         <v>0.0</v>
@@ -3655,29 +3655,29 @@
     <row r="115">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>Inductors, Coils, Chokes</t>
+          <t>Connectors</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
         <is>
-          <t>SRP4030FA-3R3M</t>
+          <t>BM06B-GHS-TBT(LF)(SN)</t>
         </is>
       </c>
       <c r="C115" s="2" t="inlineStr">
         <is>
-          <t>SMD,4.1x4.1mm</t>
+          <t>SMD,P=1.25mm</t>
         </is>
       </c>
       <c r="D115" s="2" t="inlineStr">
         <is>
-          <t>C2046796</t>
+          <t>C189892</t>
         </is>
       </c>
       <c r="E115" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F115" s="2" t="n">
-        <v>90.0</v>
+        <v>5000.0</v>
       </c>
       <c r="G115" s="2" t="n">
         <v>0.0</v>
@@ -3686,29 +3686,29 @@
     <row r="116">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>Global Sourcing Parts</t>
+          <t>Inductors, Coils, Chokes</t>
         </is>
       </c>
       <c r="B116" s="2" t="inlineStr">
         <is>
-          <t>MSD-1-A</t>
+          <t>SRP1050WA-220M</t>
         </is>
       </c>
       <c r="C116" s="2" t="inlineStr">
         <is>
-          <t>SIM-SMD</t>
+          <t>SMD,11x10mm</t>
         </is>
       </c>
       <c r="D116" s="2" t="inlineStr">
         <is>
-          <t>C20619272</t>
+          <t>C19947668</t>
         </is>
       </c>
       <c r="E116" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F116" s="2" t="n">
-        <v>90.0</v>
+        <v>30.0</v>
       </c>
       <c r="G116" s="2" t="n">
         <v>0.0</v>
@@ -3717,29 +3717,29 @@
     <row r="117">
       <c r="A117" s="2" t="inlineStr">
         <is>
-          <t>Connectors</t>
+          <t>Global Sourcing Parts</t>
         </is>
       </c>
       <c r="B117" s="2" t="inlineStr">
         <is>
-          <t>009176001884906</t>
+          <t>SRP7050WA-100M</t>
         </is>
       </c>
       <c r="C117" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>SMD,7.9x7.3mm</t>
         </is>
       </c>
       <c r="D117" s="2" t="inlineStr">
         <is>
-          <t>C20698306</t>
+          <t>C19947697</t>
         </is>
       </c>
       <c r="E117" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F117" s="2" t="n">
-        <v>120.0</v>
+        <v>90.0</v>
       </c>
       <c r="G117" s="2" t="n">
         <v>0.0</v>
@@ -3748,29 +3748,29 @@
     <row r="118">
       <c r="A118" s="2" t="inlineStr">
         <is>
-          <t>Connectors</t>
+          <t>Capacitors</t>
         </is>
       </c>
       <c r="B118" s="2" t="inlineStr">
         <is>
-          <t>ESQ-120-12-L-D</t>
+          <t>GRM155D71A475ME15J</t>
         </is>
       </c>
       <c r="C118" s="2" t="inlineStr">
         <is>
-          <t>TH-40P</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D118" s="2" t="inlineStr">
         <is>
-          <t>C20867899</t>
+          <t>C20044523</t>
         </is>
       </c>
       <c r="E118" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F118" s="2" t="n">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="G118" s="2" t="n">
         <v>0.0</v>
@@ -3779,29 +3779,29 @@
     <row r="119">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>Capacitors</t>
+          <t>Connectors</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
         <is>
-          <t>C3216X7S0J476M160AC</t>
+          <t>BM06B-GHS-TBT</t>
         </is>
       </c>
       <c r="C119" s="2" t="inlineStr">
         <is>
-          <t>1206</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D119" s="2" t="inlineStr">
         <is>
-          <t>C2167997</t>
+          <t>C20089153</t>
         </is>
       </c>
       <c r="E119" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F119" s="2" t="n">
-        <v>30.0</v>
+        <v>20.0</v>
       </c>
       <c r="G119" s="2" t="n">
         <v>0.0</v>
@@ -3810,29 +3810,29 @@
     <row r="120">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>Global Sourcing Parts</t>
+          <t>Motor Driver ICs</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
         <is>
-          <t>GSB1CA11101DSHR</t>
+          <t>DRV8849RHHR</t>
         </is>
       </c>
       <c r="C120" s="2" t="inlineStr">
         <is>
-          <t>TYPE-C</t>
+          <t>VQFN-36(6x6)</t>
         </is>
       </c>
       <c r="D120" s="2" t="inlineStr">
         <is>
-          <t>C22075645</t>
+          <t>C20345377</t>
         </is>
       </c>
       <c r="E120" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F120" s="2" t="n">
-        <v>10.0</v>
+        <v>90.0</v>
       </c>
       <c r="G120" s="2" t="n">
         <v>0.0</v>
@@ -3841,29 +3841,29 @@
     <row r="121">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>Global Sourcing Parts</t>
+          <t>Inductors, Coils, Chokes</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
         <is>
-          <t>STM32H573AII6</t>
+          <t>SRP4030FA-3R3M</t>
         </is>
       </c>
       <c r="C121" s="2" t="inlineStr">
         <is>
-          <t>BGA169-7X7-0.5</t>
+          <t>SMD,4.1x4.1mm</t>
         </is>
       </c>
       <c r="D121" s="2" t="inlineStr">
         <is>
-          <t>C22394393</t>
+          <t>C2046796</t>
         </is>
       </c>
       <c r="E121" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F121" s="2" t="n">
-        <v>45.0</v>
+        <v>90.0</v>
       </c>
       <c r="G121" s="2" t="n">
         <v>0.0</v>
@@ -3877,24 +3877,24 @@
       </c>
       <c r="B122" s="2" t="inlineStr">
         <is>
-          <t>LAN8671C2T-E/U3B</t>
+          <t>MSD-1-A</t>
         </is>
       </c>
       <c r="C122" s="2" t="inlineStr">
         <is>
-          <t>QFN24-4X4-0.5</t>
+          <t>SIM-SMD</t>
         </is>
       </c>
       <c r="D122" s="2" t="inlineStr">
         <is>
-          <t>C22394443</t>
+          <t>C20619272</t>
         </is>
       </c>
       <c r="E122" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F122" s="2" t="n">
-        <v>45.0</v>
+        <v>90.0</v>
       </c>
       <c r="G122" s="2" t="n">
         <v>0.0</v>
@@ -3903,29 +3903,29 @@
     <row r="123">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>Diodes</t>
+          <t>Connectors</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
         <is>
-          <t>MMBD1501A</t>
+          <t>009176001884906</t>
         </is>
       </c>
       <c r="C123" s="2" t="inlineStr">
         <is>
-          <t>SOT-23</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D123" s="2" t="inlineStr">
         <is>
-          <t>C236937</t>
+          <t>C20698306</t>
         </is>
       </c>
       <c r="E123" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F123" s="2" t="n">
-        <v>30.0</v>
+        <v>120.0</v>
       </c>
       <c r="G123" s="2" t="n">
         <v>0.0</v>
@@ -3934,29 +3934,29 @@
     <row r="124">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>Inductors, Coils, Chokes</t>
+          <t>Connectors</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
         <is>
-          <t>0530CDMCCDS-R47MC</t>
+          <t>ESQ-120-12-L-D</t>
         </is>
       </c>
       <c r="C124" s="2" t="inlineStr">
         <is>
-          <t>SMD,5.4x5.2mm</t>
+          <t>TH-40P</t>
         </is>
       </c>
       <c r="D124" s="2" t="inlineStr">
         <is>
-          <t>C2453428</t>
+          <t>C20867899</t>
         </is>
       </c>
       <c r="E124" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F124" s="2" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="G124" s="2" t="n">
         <v>0.0</v>
@@ -3965,29 +3965,29 @@
     <row r="125">
       <c r="A125" s="2" t="inlineStr">
         <is>
-          <t>Global Sourcing Parts</t>
+          <t>Capacitors</t>
         </is>
       </c>
       <c r="B125" s="2" t="inlineStr">
         <is>
-          <t>ACS781LLRTR-100U-T</t>
+          <t>C3216X7S0J476M160AC</t>
         </is>
       </c>
       <c r="C125" s="2" t="inlineStr">
         <is>
-          <t>PSOF-7</t>
+          <t>1206</t>
         </is>
       </c>
       <c r="D125" s="2" t="inlineStr">
         <is>
-          <t>C2654916</t>
+          <t>C2167997</t>
         </is>
       </c>
       <c r="E125" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F125" s="2" t="n">
-        <v>10.0</v>
+        <v>30.0</v>
       </c>
       <c r="G125" s="2" t="n">
         <v>0.0</v>
@@ -3996,29 +3996,29 @@
     <row r="126">
       <c r="A126" s="2" t="inlineStr">
         <is>
-          <t>LED Drivers</t>
+          <t>Global Sourcing Parts</t>
         </is>
       </c>
       <c r="B126" s="2" t="inlineStr">
         <is>
-          <t>PCA9685PW,118</t>
+          <t>GSB1CA11101DSHR</t>
         </is>
       </c>
       <c r="C126" s="2" t="inlineStr">
         <is>
-          <t>TSSOP-28</t>
+          <t>TYPE-C</t>
         </is>
       </c>
       <c r="D126" s="2" t="inlineStr">
         <is>
-          <t>C2678753</t>
+          <t>C22075645</t>
         </is>
       </c>
       <c r="E126" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F126" s="2" t="n">
-        <v>500.0</v>
+        <v>10.0</v>
       </c>
       <c r="G126" s="2" t="n">
         <v>0.0</v>
@@ -4032,24 +4032,24 @@
       </c>
       <c r="B127" s="2" t="inlineStr">
         <is>
-          <t>2026560021</t>
+          <t>STM32H573AII6</t>
         </is>
       </c>
       <c r="C127" s="2" t="inlineStr">
         <is>
-          <t>SMD-2P</t>
+          <t>BGA169-7X7-0.5</t>
         </is>
       </c>
       <c r="D127" s="2" t="inlineStr">
         <is>
-          <t>C2916937</t>
+          <t>C22394393</t>
         </is>
       </c>
       <c r="E127" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F127" s="2" t="n">
-        <v>30.0</v>
+        <v>45.0</v>
       </c>
       <c r="G127" s="2" t="n">
         <v>0.0</v>
@@ -4058,29 +4058,29 @@
     <row r="128">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>Connectors</t>
+          <t>Global Sourcing Parts</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
         <is>
-          <t>2328702-6</t>
+          <t>LAN8671C2T-E/U3B</t>
         </is>
       </c>
       <c r="C128" s="2" t="inlineStr">
         <is>
-          <t>FPC-SMD,6P,0.5mm</t>
+          <t>QFN24-4X4-0.5</t>
         </is>
       </c>
       <c r="D128" s="2" t="inlineStr">
         <is>
-          <t>C3151647</t>
+          <t>C22394443</t>
         </is>
       </c>
       <c r="E128" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F128" s="2" t="n">
-        <v>1000.0</v>
+        <v>145.0</v>
       </c>
       <c r="G128" s="2" t="n">
         <v>0.0</v>
@@ -4089,29 +4089,29 @@
     <row r="129">
       <c r="A129" s="2" t="inlineStr">
         <is>
-          <t>Power Management (PMIC)</t>
+          <t>Diodes</t>
         </is>
       </c>
       <c r="B129" s="2" t="inlineStr">
         <is>
-          <t>MAX20408AFOE/VY+</t>
+          <t>MMBD1501A</t>
         </is>
       </c>
       <c r="C129" s="2" t="inlineStr">
         <is>
-          <t>FC2QFN-17(3.5x3.8)</t>
+          <t>SOT-23</t>
         </is>
       </c>
       <c r="D129" s="2" t="inlineStr">
         <is>
-          <t>C3188488</t>
+          <t>C236937</t>
         </is>
       </c>
       <c r="E129" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F129" s="2" t="n">
-        <v>10.0</v>
+        <v>30.0</v>
       </c>
       <c r="G129" s="2" t="n">
         <v>0.0</v>
@@ -4120,29 +4120,29 @@
     <row r="130">
       <c r="A130" s="2" t="inlineStr">
         <is>
-          <t>Interface</t>
+          <t>Inductors, Coils, Chokes</t>
         </is>
       </c>
       <c r="B130" s="2" t="inlineStr">
         <is>
-          <t>88LX2730A0-NYC2C000</t>
+          <t>0530CDMCCDS-R47MC</t>
         </is>
       </c>
       <c r="C130" s="2" t="inlineStr">
         <is>
-          <t>QFN-28(4x4)</t>
+          <t>SMD,5.4x5.2mm</t>
         </is>
       </c>
       <c r="D130" s="2" t="inlineStr">
         <is>
-          <t>C3220259</t>
+          <t>C2453428</t>
         </is>
       </c>
       <c r="E130" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F130" s="2" t="n">
-        <v>40.0</v>
+        <v>10.0</v>
       </c>
       <c r="G130" s="2" t="n">
         <v>0.0</v>
@@ -4151,22 +4151,22 @@
     <row r="131">
       <c r="A131" s="2" t="inlineStr">
         <is>
-          <t>Connectors</t>
+          <t>Global Sourcing Parts</t>
         </is>
       </c>
       <c r="B131" s="2" t="inlineStr">
         <is>
-          <t>TSW-103-07-G-T</t>
+          <t>ACS781LLRTR-100U-T</t>
         </is>
       </c>
       <c r="C131" s="2" t="inlineStr">
         <is>
-          <t>插件,P=2.54mm</t>
+          <t>PSOF-7</t>
         </is>
       </c>
       <c r="D131" s="2" t="inlineStr">
         <is>
-          <t>C3332322</t>
+          <t>C2654916</t>
         </is>
       </c>
       <c r="E131" s="2" t="n">
@@ -4182,29 +4182,29 @@
     <row r="132">
       <c r="A132" s="2" t="inlineStr">
         <is>
-          <t>Logic</t>
+          <t>LED Drivers</t>
         </is>
       </c>
       <c r="B132" s="2" t="inlineStr">
         <is>
-          <t>TXS0102YZPR</t>
+          <t>PCA9685PW,118</t>
         </is>
       </c>
       <c r="C132" s="2" t="inlineStr">
         <is>
-          <t>DSBGA-8</t>
+          <t>TSSOP-28</t>
         </is>
       </c>
       <c r="D132" s="2" t="inlineStr">
         <is>
-          <t>C353037</t>
+          <t>C2678753</t>
         </is>
       </c>
       <c r="E132" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F132" s="2" t="n">
-        <v>3000.0</v>
+        <v>500.0</v>
       </c>
       <c r="G132" s="2" t="n">
         <v>0.0</v>
@@ -4213,29 +4213,29 @@
     <row r="133">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>Optoelectronics</t>
+          <t>Global Sourcing Parts</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
         <is>
-          <t>LTST-S270TGKT</t>
+          <t>2026560021</t>
         </is>
       </c>
       <c r="C133" s="2" t="inlineStr">
         <is>
-          <t>SMD,1.2x1.6mm</t>
+          <t>SMD-2P</t>
         </is>
       </c>
       <c r="D133" s="2" t="inlineStr">
         <is>
-          <t>C364567</t>
+          <t>C2916937</t>
         </is>
       </c>
       <c r="E133" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F133" s="2" t="n">
-        <v>1500.0</v>
+        <v>30.0</v>
       </c>
       <c r="G133" s="2" t="n">
         <v>0.0</v>
@@ -4249,24 +4249,24 @@
       </c>
       <c r="B134" s="2" t="inlineStr">
         <is>
-          <t>284093-6</t>
+          <t>2328702-6</t>
         </is>
       </c>
       <c r="C134" s="2" t="inlineStr">
         <is>
-          <t>插件,P=5mm</t>
+          <t>FPC-SMD,6P,0.5mm</t>
         </is>
       </c>
       <c r="D134" s="2" t="inlineStr">
         <is>
-          <t>C3818250</t>
+          <t>C3151647</t>
         </is>
       </c>
       <c r="E134" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F134" s="2" t="n">
-        <v>20.0</v>
+        <v>1000.0</v>
       </c>
       <c r="G134" s="2" t="n">
         <v>0.0</v>
@@ -4275,29 +4275,29 @@
     <row r="135">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>Resistors</t>
+          <t>Power Management (PMIC)</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
         <is>
-          <t>RC0402FR-071K15L</t>
+          <t>MAX20408AFOE/VY+</t>
         </is>
       </c>
       <c r="C135" s="2" t="inlineStr">
         <is>
-          <t>0402</t>
+          <t>FC2QFN-17(3.5x3.8)</t>
         </is>
       </c>
       <c r="D135" s="2" t="inlineStr">
         <is>
-          <t>C477191</t>
+          <t>C3188488</t>
         </is>
       </c>
       <c r="E135" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F135" s="2" t="n">
-        <v>2500.0</v>
+        <v>10.0</v>
       </c>
       <c r="G135" s="2" t="n">
         <v>0.0</v>
@@ -4306,29 +4306,29 @@
     <row r="136">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>Resistors</t>
+          <t>Interface</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
         <is>
-          <t>RC0402FR-0719K6L</t>
+          <t>88LX2730A0-NYC2C000</t>
         </is>
       </c>
       <c r="C136" s="2" t="inlineStr">
         <is>
-          <t>0402</t>
+          <t>QFN-28(4x4)</t>
         </is>
       </c>
       <c r="D136" s="2" t="inlineStr">
         <is>
-          <t>C477629</t>
+          <t>C3220259</t>
         </is>
       </c>
       <c r="E136" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F136" s="2" t="n">
-        <v>1000.0</v>
+        <v>40.0</v>
       </c>
       <c r="G136" s="2" t="n">
         <v>0.0</v>
@@ -4337,29 +4337,29 @@
     <row r="137">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>Global Sourcing Parts</t>
+          <t>Connectors</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
         <is>
-          <t>0532610471</t>
+          <t>TSW-103-07-G-T</t>
         </is>
       </c>
       <c r="C137" s="2" t="inlineStr">
         <is>
-          <t>SMD-4P</t>
+          <t>插件,P=2.54mm</t>
         </is>
       </c>
       <c r="D137" s="2" t="inlineStr">
         <is>
-          <t>C5119769</t>
+          <t>C3332322</t>
         </is>
       </c>
       <c r="E137" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F137" s="2" t="n">
-        <v>100.0</v>
+        <v>10.0</v>
       </c>
       <c r="G137" s="2" t="n">
         <v>0.0</v>
@@ -4368,29 +4368,29 @@
     <row r="138">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>Global Sourcing Parts</t>
+          <t>Logic</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
         <is>
-          <t>BMP390</t>
+          <t>TXS0102YZPR</t>
         </is>
       </c>
       <c r="C138" s="2" t="inlineStr">
         <is>
-          <t>LGA-10(2x2)</t>
+          <t>DSBGA-8</t>
         </is>
       </c>
       <c r="D138" s="2" t="inlineStr">
         <is>
-          <t>C5124834</t>
+          <t>C353037</t>
         </is>
       </c>
       <c r="E138" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F138" s="2" t="n">
-        <v>500.0</v>
+        <v>3000.0</v>
       </c>
       <c r="G138" s="2" t="n">
         <v>0.0</v>
@@ -4399,29 +4399,29 @@
     <row r="139">
       <c r="A139" s="2" t="inlineStr">
         <is>
-          <t>Motor Driver ICs</t>
+          <t>Optoelectronics</t>
         </is>
       </c>
       <c r="B139" s="2" t="inlineStr">
         <is>
-          <t>DRV8311HRRWR</t>
+          <t>LTST-S270TGKT</t>
         </is>
       </c>
       <c r="C139" s="2" t="inlineStr">
         <is>
-          <t>WQFN(RRW)-24</t>
+          <t>SMD,1.2x1.6mm</t>
         </is>
       </c>
       <c r="D139" s="2" t="inlineStr">
         <is>
-          <t>C5218862</t>
+          <t>C364567</t>
         </is>
       </c>
       <c r="E139" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F139" s="2" t="n">
-        <v>15.0</v>
+        <v>1500.0</v>
       </c>
       <c r="G139" s="2" t="n">
         <v>0.0</v>
@@ -4430,29 +4430,29 @@
     <row r="140">
       <c r="A140" s="2" t="inlineStr">
         <is>
-          <t>Global Sourcing Parts</t>
+          <t>Connectors</t>
         </is>
       </c>
       <c r="B140" s="2" t="inlineStr">
         <is>
-          <t>009176001853906</t>
+          <t>284093-6</t>
         </is>
       </c>
       <c r="C140" s="2" t="inlineStr">
         <is>
-          <t>SMD</t>
+          <t>插件,P=5mm</t>
         </is>
       </c>
       <c r="D140" s="2" t="inlineStr">
         <is>
-          <t>C5354438</t>
+          <t>C3818250</t>
         </is>
       </c>
       <c r="E140" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F140" s="2" t="n">
-        <v>240.0</v>
+        <v>20.0</v>
       </c>
       <c r="G140" s="2" t="n">
         <v>0.0</v>
@@ -4461,29 +4461,29 @@
     <row r="141">
       <c r="A141" s="2" t="inlineStr">
         <is>
-          <t>Connectors</t>
+          <t>Resistors</t>
         </is>
       </c>
       <c r="B141" s="2" t="inlineStr">
         <is>
-          <t>5034801600</t>
+          <t>RC0402FR-071K15L</t>
         </is>
       </c>
       <c r="C141" s="2" t="inlineStr">
         <is>
-          <t>SMD,P=0.5mm,卧贴</t>
+          <t>0402</t>
         </is>
       </c>
       <c r="D141" s="2" t="inlineStr">
         <is>
-          <t>C5510131</t>
+          <t>C477191</t>
         </is>
       </c>
       <c r="E141" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F141" s="2" t="n">
-        <v>89.0</v>
+        <v>2500.0</v>
       </c>
       <c r="G141" s="2" t="n">
         <v>0.0</v>
@@ -4492,29 +4492,29 @@
     <row r="142">
       <c r="A142" s="2" t="inlineStr">
         <is>
-          <t>Optoelectronics</t>
+          <t>Resistors</t>
         </is>
       </c>
       <c r="B142" s="2" t="inlineStr">
         <is>
-          <t>APDA1806ZGCK</t>
+          <t>RC0402FR-0719K6L</t>
         </is>
       </c>
       <c r="C142" s="2" t="inlineStr">
         <is>
-          <t>SMD</t>
+          <t>0402</t>
         </is>
       </c>
       <c r="D142" s="2" t="inlineStr">
         <is>
-          <t>C5568685</t>
+          <t>C477629</t>
         </is>
       </c>
       <c r="E142" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F142" s="2" t="n">
-        <v>10.0</v>
+        <v>1000.0</v>
       </c>
       <c r="G142" s="2" t="n">
         <v>0.0</v>
@@ -4523,29 +4523,29 @@
     <row r="143">
       <c r="A143" s="2" t="inlineStr">
         <is>
-          <t>Connectors</t>
+          <t>Global Sourcing Parts</t>
         </is>
       </c>
       <c r="B143" s="2" t="inlineStr">
         <is>
-          <t>47615-0001</t>
+          <t>0532610471</t>
         </is>
       </c>
       <c r="C143" s="2" t="inlineStr">
         <is>
-          <t>SMD</t>
+          <t>SMD-4P</t>
         </is>
       </c>
       <c r="D143" s="2" t="inlineStr">
         <is>
-          <t>C5727183</t>
+          <t>C5119769</t>
         </is>
       </c>
       <c r="E143" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F143" s="2" t="n">
-        <v>80.0</v>
+        <v>100.0</v>
       </c>
       <c r="G143" s="2" t="n">
         <v>0.0</v>
@@ -4554,29 +4554,29 @@
     <row r="144">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>Resistors</t>
+          <t>Global Sourcing Parts</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
         <is>
-          <t>PE0805FRE470R009Z</t>
+          <t>BMP390</t>
         </is>
       </c>
       <c r="C144" s="2" t="inlineStr">
         <is>
-          <t>0805</t>
+          <t>LGA-10(2x2)</t>
         </is>
       </c>
       <c r="D144" s="2" t="inlineStr">
         <is>
-          <t>C6142798</t>
+          <t>C5124834</t>
         </is>
       </c>
       <c r="E144" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F144" s="2" t="n">
-        <v>30.0</v>
+        <v>500.0</v>
       </c>
       <c r="G144" s="2" t="n">
         <v>0.0</v>
@@ -4585,29 +4585,29 @@
     <row r="145">
       <c r="A145" s="2" t="inlineStr">
         <is>
-          <t>Amplifiers/Comparators</t>
+          <t>Motor Driver ICs</t>
         </is>
       </c>
       <c r="B145" s="2" t="inlineStr">
         <is>
-          <t>MCP6002T-E/MC</t>
+          <t>DRV8311HRRWR</t>
         </is>
       </c>
       <c r="C145" s="2" t="inlineStr">
         <is>
-          <t>DFN-8-EP(2x3)</t>
+          <t>WQFN(RRW)-24</t>
         </is>
       </c>
       <c r="D145" s="2" t="inlineStr">
         <is>
-          <t>C623660</t>
+          <t>C5218862</t>
         </is>
       </c>
       <c r="E145" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F145" s="2" t="n">
-        <v>30.0</v>
+        <v>15.0</v>
       </c>
       <c r="G145" s="2" t="n">
         <v>0.0</v>
@@ -4616,29 +4616,29 @@
     <row r="146">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>Connectors</t>
+          <t>Global Sourcing Parts</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
         <is>
-          <t>MTSW-116-23-L-T-230</t>
+          <t>009176001853906</t>
         </is>
       </c>
       <c r="C146" s="2" t="inlineStr">
         <is>
-          <t>插件,P=2.54mm</t>
+          <t>SMD</t>
         </is>
       </c>
       <c r="D146" s="2" t="inlineStr">
         <is>
-          <t>C6609190</t>
+          <t>C5354438</t>
         </is>
       </c>
       <c r="E146" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F146" s="2" t="n">
-        <v>6.0</v>
+        <v>240.0</v>
       </c>
       <c r="G146" s="2" t="n">
         <v>0.0</v>
@@ -4652,24 +4652,24 @@
       </c>
       <c r="B147" s="2" t="inlineStr">
         <is>
-          <t>TSW-103-07-T-T</t>
+          <t>5034801600</t>
         </is>
       </c>
       <c r="C147" s="2" t="inlineStr">
         <is>
-          <t>插件,P=2.54mm,3x3P</t>
+          <t>SMD,P=0.5mm,卧贴</t>
         </is>
       </c>
       <c r="D147" s="2" t="inlineStr">
         <is>
-          <t>C7074299</t>
+          <t>C5510131</t>
         </is>
       </c>
       <c r="E147" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F147" s="2" t="n">
-        <v>500.0</v>
+        <v>89.0</v>
       </c>
       <c r="G147" s="2" t="n">
         <v>0.0</v>
@@ -4678,29 +4678,29 @@
     <row r="148">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>Transistors/Thyristors</t>
+          <t>Optoelectronics</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
         <is>
-          <t>SQJ974EP-T1_GE3</t>
+          <t>APDA1806ZGCK</t>
         </is>
       </c>
       <c r="C148" s="2" t="inlineStr">
         <is>
-          <t>PowerPAK-SO-8-4</t>
+          <t>SMD</t>
         </is>
       </c>
       <c r="D148" s="2" t="inlineStr">
         <is>
-          <t>C727845</t>
+          <t>C5568685</t>
         </is>
       </c>
       <c r="E148" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F148" s="2" t="n">
-        <v>30.0</v>
+        <v>10.0</v>
       </c>
       <c r="G148" s="2" t="n">
         <v>0.0</v>
@@ -4709,29 +4709,29 @@
     <row r="149">
       <c r="A149" s="2" t="inlineStr">
         <is>
-          <t>Power Management (PMIC)</t>
+          <t>Connectors</t>
         </is>
       </c>
       <c r="B149" s="2" t="inlineStr">
         <is>
-          <t>MIC5365-3.3YC5-TR</t>
+          <t>47615-0001</t>
         </is>
       </c>
       <c r="C149" s="2" t="inlineStr">
         <is>
-          <t>SC-70-5</t>
+          <t>SMD</t>
         </is>
       </c>
       <c r="D149" s="2" t="inlineStr">
         <is>
-          <t>C73103</t>
+          <t>C5727183</t>
         </is>
       </c>
       <c r="E149" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F149" s="2" t="n">
-        <v>10.0</v>
+        <v>80.0</v>
       </c>
       <c r="G149" s="2" t="n">
         <v>0.0</v>
@@ -4740,22 +4740,22 @@
     <row r="150">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>Power Management (PMIC)</t>
+          <t>Resistors</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
         <is>
-          <t>LM5122MHX/NOPB</t>
+          <t>PE0805FRE470R009Z</t>
         </is>
       </c>
       <c r="C150" s="2" t="inlineStr">
         <is>
-          <t>HTSSOP-20-EP</t>
+          <t>0805</t>
         </is>
       </c>
       <c r="D150" s="2" t="inlineStr">
         <is>
-          <t>C77241</t>
+          <t>C6142798</t>
         </is>
       </c>
       <c r="E150" s="2" t="n">
@@ -4771,29 +4771,29 @@
     <row r="151">
       <c r="A151" s="2" t="inlineStr">
         <is>
-          <t>Capacitors</t>
+          <t>Amplifiers/Comparators</t>
         </is>
       </c>
       <c r="B151" s="2" t="inlineStr">
         <is>
-          <t>GRM155R71A474KE01D</t>
+          <t>MCP6002T-E/MC</t>
         </is>
       </c>
       <c r="C151" s="2" t="inlineStr">
         <is>
-          <t>0402</t>
+          <t>DFN-8-EP(2x3)</t>
         </is>
       </c>
       <c r="D151" s="2" t="inlineStr">
         <is>
-          <t>C88946</t>
+          <t>C623660</t>
         </is>
       </c>
       <c r="E151" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F151" s="2" t="n">
-        <v>10.0</v>
+        <v>30.0</v>
       </c>
       <c r="G151" s="2" t="n">
         <v>0.0</v>
@@ -4802,29 +4802,29 @@
     <row r="152">
       <c r="A152" s="2" t="inlineStr">
         <is>
-          <t>Resistors</t>
+          <t>Connectors</t>
         </is>
       </c>
       <c r="B152" s="2" t="inlineStr">
         <is>
-          <t>RC0402FR-0720KL</t>
+          <t>MTSW-116-23-L-T-230</t>
         </is>
       </c>
       <c r="C152" s="2" t="inlineStr">
         <is>
-          <t>0402</t>
+          <t>插件,P=2.54mm</t>
         </is>
       </c>
       <c r="D152" s="2" t="inlineStr">
         <is>
-          <t>C93942</t>
+          <t>C6609190</t>
         </is>
       </c>
       <c r="E152" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F152" s="2" t="n">
-        <v>1000.0</v>
+        <v>6.0</v>
       </c>
       <c r="G152" s="2" t="n">
         <v>0.0</v>
@@ -4833,62 +4833,248 @@
     <row r="153">
       <c r="A153" s="2" t="inlineStr">
         <is>
-          <t>Others</t>
+          <t>Connectors</t>
         </is>
       </c>
       <c r="B153" s="2" t="inlineStr">
         <is>
-          <t>Part number 15872</t>
+          <t>TSW-103-07-T-T</t>
         </is>
       </c>
       <c r="C153" s="2" t="inlineStr">
         <is>
-          <t>插件,P=2.54mm,3x16P</t>
+          <t>插件,P=2.54mm,3x3P</t>
         </is>
       </c>
       <c r="D153" s="2" t="inlineStr">
         <is>
-          <t>C9900147096</t>
+          <t>C7074299</t>
         </is>
       </c>
       <c r="E153" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="F153" s="2" t="n">
-        <v>0.0</v>
+        <v>500.0</v>
       </c>
       <c r="G153" s="2" t="n">
-        <v>1000.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="2" t="inlineStr">
         <is>
+          <t>Transistors/Thyristors</t>
+        </is>
+      </c>
+      <c r="B154" s="2" t="inlineStr">
+        <is>
+          <t>SQJ974EP-T1_GE3</t>
+        </is>
+      </c>
+      <c r="C154" s="2" t="inlineStr">
+        <is>
+          <t>PowerPAK-SO-8-4</t>
+        </is>
+      </c>
+      <c r="D154" s="2" t="inlineStr">
+        <is>
+          <t>C727845</t>
+        </is>
+      </c>
+      <c r="E154" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F154" s="2" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="G154" s="2" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="2" t="inlineStr">
+        <is>
+          <t>Power Management (PMIC)</t>
+        </is>
+      </c>
+      <c r="B155" s="2" t="inlineStr">
+        <is>
+          <t>MIC5365-3.3YC5-TR</t>
+        </is>
+      </c>
+      <c r="C155" s="2" t="inlineStr">
+        <is>
+          <t>SC-70-5</t>
+        </is>
+      </c>
+      <c r="D155" s="2" t="inlineStr">
+        <is>
+          <t>C73103</t>
+        </is>
+      </c>
+      <c r="E155" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F155" s="2" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G155" s="2" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="2" t="inlineStr">
+        <is>
+          <t>Power Management (PMIC)</t>
+        </is>
+      </c>
+      <c r="B156" s="2" t="inlineStr">
+        <is>
+          <t>LM5122MHX/NOPB</t>
+        </is>
+      </c>
+      <c r="C156" s="2" t="inlineStr">
+        <is>
+          <t>HTSSOP-20-EP</t>
+        </is>
+      </c>
+      <c r="D156" s="2" t="inlineStr">
+        <is>
+          <t>C77241</t>
+        </is>
+      </c>
+      <c r="E156" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F156" s="2" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="G156" s="2" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="2" t="inlineStr">
+        <is>
+          <t>Capacitors</t>
+        </is>
+      </c>
+      <c r="B157" s="2" t="inlineStr">
+        <is>
+          <t>GRM155R71A474KE01D</t>
+        </is>
+      </c>
+      <c r="C157" s="2" t="inlineStr">
+        <is>
+          <t>0402</t>
+        </is>
+      </c>
+      <c r="D157" s="2" t="inlineStr">
+        <is>
+          <t>C88946</t>
+        </is>
+      </c>
+      <c r="E157" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F157" s="2" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G157" s="2" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="2" t="inlineStr">
+        <is>
+          <t>Resistors</t>
+        </is>
+      </c>
+      <c r="B158" s="2" t="inlineStr">
+        <is>
+          <t>RC0402FR-0720KL</t>
+        </is>
+      </c>
+      <c r="C158" s="2" t="inlineStr">
+        <is>
+          <t>0402</t>
+        </is>
+      </c>
+      <c r="D158" s="2" t="inlineStr">
+        <is>
+          <t>C93942</t>
+        </is>
+      </c>
+      <c r="E158" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F158" s="2" t="n">
+        <v>1000.0</v>
+      </c>
+      <c r="G158" s="2" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="2" t="inlineStr">
+        <is>
           <t>Others</t>
         </is>
       </c>
-      <c r="B154" s="2" t="inlineStr">
+      <c r="B159" s="2" t="inlineStr">
+        <is>
+          <t>Part number 15872</t>
+        </is>
+      </c>
+      <c r="C159" s="2" t="inlineStr">
+        <is>
+          <t>插件,P=2.54mm,3x16P</t>
+        </is>
+      </c>
+      <c r="D159" s="2" t="inlineStr">
+        <is>
+          <t>C9900147096</t>
+        </is>
+      </c>
+      <c r="E159" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F159" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G159" s="2" t="n">
+        <v>1000.0</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="2" t="inlineStr">
+        <is>
+          <t>Others</t>
+        </is>
+      </c>
+      <c r="B160" s="2" t="inlineStr">
         <is>
           <t>Part number 15379</t>
         </is>
       </c>
-      <c r="C154" s="2" t="inlineStr">
+      <c r="C160" s="2" t="inlineStr">
         <is>
           <t>插件,P=2.54mm,2x20P</t>
         </is>
       </c>
-      <c r="D154" s="2" t="inlineStr">
+      <c r="D160" s="2" t="inlineStr">
         <is>
           <t>C9900147097</t>
         </is>
       </c>
-      <c r="E154" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F154" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G154" s="2" t="n">
+      <c r="E160" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F160" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G160" s="2" t="n">
         <v>1000.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
I can't even begin with the changes, mainly added a remove all BREs function, added a sort field to Odoo, small edits elsewhere
</commit_message>
<xml_diff>
--- a/jlc-scraper/csv/Parts Inventory on JLCPCB.xlsx
+++ b/jlc-scraper/csv/Parts Inventory on JLCPCB.xlsx
@@ -1504,7 +1504,7 @@
         </is>
       </c>
       <c r="E45" s="2" t="n">
-        <v>0.0</v>
+        <v>3834.0</v>
       </c>
       <c r="F45" s="2" t="n">
         <v>0.0</v>
@@ -1535,7 +1535,7 @@
         </is>
       </c>
       <c r="E46" s="2" t="n">
-        <v>0.0</v>
+        <v>3834.0</v>
       </c>
       <c r="F46" s="2" t="n">
         <v>0.0</v>
@@ -3271,7 +3271,7 @@
         </is>
       </c>
       <c r="E102" s="2" t="n">
-        <v>0.0</v>
+        <v>2517.0</v>
       </c>
       <c r="F102" s="2" t="n">
         <v>0.0</v>

</xml_diff>

<commit_message>
Lots of updates to code, probably should've pushed awhile ago
</commit_message>
<xml_diff>
--- a/jlc-scraper/csv/Parts Inventory on JLCPCB.xlsx
+++ b/jlc-scraper/csv/Parts Inventory on JLCPCB.xlsx
@@ -202,7 +202,7 @@
         </is>
       </c>
       <c r="E3" s="2" t="n">
-        <v>9615.0</v>
+        <v>9230.0</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>0.0</v>
@@ -326,7 +326,7 @@
         </is>
       </c>
       <c r="E7" s="2" t="n">
-        <v>1740.0</v>
+        <v>480.0</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>0.0</v>
@@ -357,7 +357,7 @@
         </is>
       </c>
       <c r="E8" s="2" t="n">
-        <v>3220.0</v>
+        <v>1960.0</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>0.0</v>
@@ -388,7 +388,7 @@
         </is>
       </c>
       <c r="E9" s="2" t="n">
-        <v>9115.0</v>
+        <v>8230.0</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>0.0</v>
@@ -946,7 +946,7 @@
         </is>
       </c>
       <c r="E27" s="2" t="n">
-        <v>865.0</v>
+        <v>730.0</v>
       </c>
       <c r="F27" s="2" t="n">
         <v>0.0</v>
@@ -1008,7 +1008,7 @@
         </is>
       </c>
       <c r="E29" s="2" t="n">
-        <v>2000.0</v>
+        <v>0.0</v>
       </c>
       <c r="F29" s="2" t="n">
         <v>0.0</v>
@@ -1194,7 +1194,7 @@
         </is>
       </c>
       <c r="E35" s="2" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="F35" s="2" t="n">
         <v>0.0</v>
@@ -1225,7 +1225,7 @@
         </is>
       </c>
       <c r="E36" s="2" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="F36" s="2" t="n">
         <v>28.0</v>
@@ -2031,7 +2031,7 @@
         </is>
       </c>
       <c r="E62" s="2" t="n">
-        <v>280.0</v>
+        <v>155.0</v>
       </c>
       <c r="F62" s="2" t="n">
         <v>0.0</v>
@@ -2713,7 +2713,7 @@
         </is>
       </c>
       <c r="E84" s="2" t="n">
-        <v>9.0</v>
+        <v>0.0</v>
       </c>
       <c r="F84" s="2" t="n">
         <v>0.0</v>
@@ -2961,7 +2961,7 @@
         </is>
       </c>
       <c r="E92" s="2" t="n">
-        <v>75.0</v>
+        <v>0.0</v>
       </c>
       <c r="F92" s="2" t="n">
         <v>0.0</v>
@@ -3333,7 +3333,7 @@
         </is>
       </c>
       <c r="E104" s="2" t="n">
-        <v>350.0</v>
+        <v>225.0</v>
       </c>
       <c r="F104" s="2" t="n">
         <v>0.0</v>

</xml_diff>